<commit_message>
data cleanup continued in player_per_game_df
</commit_message>
<xml_diff>
--- a/dpoy_pivot_table.xlsx
+++ b/dpoy_pivot_table.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>player</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>Hakeem Olajuwon</t>
-  </si>
-  <si>
-    <t>Jaren Jackson Jr.</t>
   </si>
   <si>
     <t>Joakim Noah</t>
@@ -452,7 +449,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -567,7 +564,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -575,7 +572,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -607,7 +604,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -615,7 +612,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -639,7 +636,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -647,7 +644,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -655,14 +652,6 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26">
         <v>1</v>
       </c>
     </row>

</xml_diff>